<commit_message>
Project Example 1 - Bank Rating is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
+++ b/DESIGN/rules/Example 1 - Bank Rating/Bank Rating.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\openl-tablets-demo-5.24.0\apache-tomcat-9.0.41\openl-demo\user-workspace\DEFAULT\Example 1 - Bank Rating\"/>
     </mc:Choice>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="694">
   <si>
     <t>&gt; 51</t>
   </si>
@@ -4091,6 +4091,9 @@
   </si>
   <si>
     <t>= $LimitIndex * MaxLimit</t>
+  </si>
+  <si>
+    <t>Calculate Capital Dynamic (%)1</t>
   </si>
 </sst>
 </file>
@@ -4189,7 +4192,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="0" rgb="FFFFFF"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
@@ -4224,7 +4227,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="2" tint="-0.749992370372631"/>
+      <color theme="2" tint="-0.749992370372631" rgb="EEECE1"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
       <charset val="204"/>
@@ -4317,19 +4320,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
+        <fgColor theme="4" tint="-0.249977111117893" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
+        <fgColor theme="6" tint="-0.249977111117893" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4341,7 +4344,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4353,13 +4356,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2" rgb="EEECE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4371,7 +4374,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5425,7 +5428,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5436,7 +5439,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5449,7 +5452,7 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5874,10 +5877,10 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -6157,11 +6160,11 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -6174,7 +6177,7 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color theme="2" tint="-0.249977111117893" rgb="EEECE1"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -6398,13 +6401,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="3"/>
   </cellStyleXfs>
   <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -6426,13 +6427,13 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6501,7 +6502,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="5"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3"/>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6514,14 +6515,14 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="62" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="5" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6742,7 +6743,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="143" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="144" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="144" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="145" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="146" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="121" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7141,13 +7142,11 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Heading 1" xfId="5" builtinId="16"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 7" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal_EPLI rater" xfId="1" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Обычный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -7582,17 +7581,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="4" collapsed="1"/>
-    <col min="2" max="2" width="9.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="25.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.33203125" style="4" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="76.6640625" style="4" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="5.88671875" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.109375" style="4" collapsed="1"/>
+    <col min="1" max="1" style="4" width="9.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="4" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="4" width="8.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="16.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="4" width="25.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="4" width="42.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="4" width="76.6640625" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="4" width="5.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="25.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="4" width="19.109375" collapsed="true"/>
+    <col min="12" max="16384" style="4" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.35">
@@ -8133,7 +8132,7 @@
       </c>
       <c r="E57" s="183"/>
       <c r="F57" s="104" t="s">
-        <v>111</v>
+        <v>693</v>
       </c>
       <c r="G57" s="97" t="s">
         <v>571</v>
@@ -8602,9 +8601,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -8789,9 +8788,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -8920,8 +8919,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -9028,18 +9027,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="3.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="12.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="4.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="3.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="44.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -9551,9 +9550,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -9640,11 +9639,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="2" collapsed="1"/>
-    <col min="3" max="3" width="18.21875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="18.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="13.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="14.0" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
@@ -9716,8 +9715,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="28.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="76.21875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="76.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.35">
@@ -9887,8 +9886,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20.44140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -9972,10 +9971,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="2" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="2" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="17.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="39.109375" collapsed="true"/>
+    <col min="5" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -10399,10 +10398,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.109375" style="2" collapsed="1"/>
-    <col min="4" max="4" width="34.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="3" style="2" width="9.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="34.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="30.0" collapsed="true"/>
+    <col min="6" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -10799,9 +10798,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -11073,27 +11072,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.44140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="51.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="32.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="48.5546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="29.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="12.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.6640625" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="25.88671875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25" style="2" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="38.6640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="23.109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.44140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="21" max="16384" width="9.109375" style="2" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="3.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="19.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="21.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="28.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="51.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="30.109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="32.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="48.5546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="29.88671875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="2" width="9.6640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="10.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="2" width="12.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="21.6640625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="25.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="2" width="25.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="38.6640625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="2" width="23.109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="19.44140625" collapsed="true"/>
+    <col min="21" max="16384" style="2" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -12309,10 +12308,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3" collapsed="1"/>
-    <col min="3" max="3" width="43.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="3" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="43.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.35">
@@ -13031,10 +13030,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -13131,9 +13130,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="26.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -13437,9 +13436,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -13545,8 +13544,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="31.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -13914,9 +13913,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" customWidth="true" width="18.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -14083,12 +14082,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="14" collapsed="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" style="14" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="44.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="40.44140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="26.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>